<commit_message>
feat: Implement new application submission pages and API endpoint, clean up temporary web app files, and update competition scripts.
</commit_message>
<xml_diff>
--- a/oylama_sonuclari.xlsx
+++ b/oylama_sonuclari.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="120">
   <si>
     <t>photoId</t>
   </si>
@@ -31,25 +31,349 @@
     <t>timestamp</t>
   </si>
   <si>
+    <t>YARISMA_ID_001</t>
+  </si>
+  <si>
     <t>YARISMA_ID_002</t>
   </si>
   <si>
-    <t>YARISMA_ID_055</t>
-  </si>
-  <si>
-    <t>YARISMA_ID_109</t>
-  </si>
-  <si>
-    <t>inlhalk@gmail.com</t>
-  </si>
-  <si>
-    <t>2026-01-05 23:01:18</t>
-  </si>
-  <si>
-    <t>2026-01-05 23:03:34</t>
-  </si>
-  <si>
-    <t>2026-01-05 23:03:39</t>
+    <t>YARISMA_ID_003</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_004</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_005</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_006</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_008</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_009</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_010</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_011</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_012</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_013</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_014</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_015</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_018</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_019</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_020</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_024</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_025</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_026</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_027</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_028</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_032</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_035</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_036</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_037</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_040</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_041</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_042</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_043</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_044</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_045</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_046</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_047</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_048</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_050</t>
+  </si>
+  <si>
+    <t>YARISMA_ID_051</t>
+  </si>
+  <si>
+    <t>ahmet.bitirim@yuzuncuyil.juri</t>
+  </si>
+  <si>
+    <t>amil.ucbas@yuzuncuyil.juri</t>
+  </si>
+  <si>
+    <t>haluk.inal@yuzuncuyil.juri</t>
+  </si>
+  <si>
+    <t>salim.karaboga@yuzunciyil.juri</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:46:22</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:07:53</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:14:16</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:36:50</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:46:58</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:08:14</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:30</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:33:07</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:33:24</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:47:09</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:22:33</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:47:25</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:22:40</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:04</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:32:53</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:47:45</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:22:53</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:51:16</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:20:28</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:45</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:23:09</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:52</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:34:26</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:19:56</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:23:20</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:11:11</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:11:20</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:23:31</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:39:23</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:42:54</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:23:42</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:11</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:48:42</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:33</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:23:50</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:48:49</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:24:02</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:12:35</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:33:54</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:24:12</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:23:49</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:17:18</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:35:35</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:20:07</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:35:50</t>
+  </si>
+  <si>
+    <t>2026-01-09 13:55:52</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:19:50</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:20</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:33:15</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:37</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:25</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:37:18</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:41:55</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:17:12</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:39:04</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:12:28</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:22:23</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:25</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:01</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:47</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:20:17</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:09:57</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:40:32</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:15</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:10</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:18</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:27</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:10:30</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:36:25</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:35</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:13:24</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:35:26</t>
+  </si>
+  <si>
+    <t>2026-01-09 14:02:54</t>
+  </si>
+  <si>
+    <t>2026-01-09 16:25:57</t>
   </si>
 </sst>
 </file>
@@ -407,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,41 +759,1035 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>11</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>43</v>
+      </c>
+      <c r="E62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>43</v>
+      </c>
+      <c r="E72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>